<commit_message>
update nos & annuaire dependencies f8da08e56b0cd2fbad29eaa3dad0299ca412ac10
</commit_message>
<xml_diff>
--- a/ig/nr-update/StructureDefinition-cds-bundle-response-recherche.xlsx
+++ b/ig/nr-update/StructureDefinition-cds-bundle-response-recherche.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10972" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10972" uniqueCount="574">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-07T13:30:52+00:00</t>
+    <t>2024-02-07T13:43:56+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1471,7 +1471,7 @@
     <t>Bundle.entry:practitioneRoleOrg.resource</t>
   </si>
   <si>
-    <t xml:space="preserve">PractitionerRole {https://apifhir.annuaire.sante.fr/ws-sync/exposed/structuredefinition/practitionerRole-organizationalRole-rass}
+    <t xml:space="preserve">PractitionerRole {https://interop.esante.gouv.fr/ig/fhir/annuaire/StructureDefinition/as-practitionerrole}
 </t>
   </si>
   <si>
@@ -1562,107 +1562,113 @@
     <t>Bundle.entry:practitioneRoleOrg.response.outcome</t>
   </si>
   <si>
-    <t>Bundle.entry:practitionerRolePro</t>
-  </si>
-  <si>
-    <t>practitionerRolePro</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.link</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.fullUrl</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.resource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PractitionerRole {https://apifhir.annuaire.sante.fr/ws-sync/exposed/structuredefinition/practitionerRole-professionalRole-rass}
+    <t>Bundle.entry:practitionerPro</t>
+  </si>
+  <si>
+    <t>practitionerPro</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.link</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.fullUrl</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practitioner {https://interop.esante.gouv.fr/ig/fhir/annuaire/StructureDefinition/as-practitioner}
 </t>
   </si>
   <si>
-    <t>Bundle.entry:practitionerRolePro.search</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.search.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.search.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.search.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.search.mode</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.search.score</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.request</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.request.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.request.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.request.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.request.method</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.request.url</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.request.ifNoneMatch</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.request.ifModifiedSince</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.request.ifMatch</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.request.ifNoneExist</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.response</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.response.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.response.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.response.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.response.status</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.response.location</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.response.etag</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.response.lastModified</t>
-  </si>
-  <si>
-    <t>Bundle.entry:practitionerRolePro.response.outcome</t>
+    <t>A person with a  formal responsibility in the provisioning of healthcare or related services | Prestataire de santé</t>
+  </si>
+  <si>
+    <t>A person who is directly or indirectly involved in the provisioning of healthcare | Un professionnel impliqué directement ou indirectement dans la prise en charge d'une personne.</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.search</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.search.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.search.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.search.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.search.mode</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.search.score</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.request</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.request.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.request.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.request.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.request.method</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.request.url</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.request.ifNoneMatch</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.request.ifModifiedSince</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.request.ifMatch</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.request.ifNoneExist</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.response</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.response.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.response.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.response.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.response.status</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.response.location</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.response.etag</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.response.lastModified</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerPro.response.outcome</t>
   </si>
   <si>
     <t>Bundle.entry:practitioner</t>
@@ -1687,16 +1693,6 @@
   </si>
   <si>
     <t>Bundle.entry:practitioner.resource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Practitioner {http://interopsante.org/fhir/StructureDefinition/FrPractitioner}
-</t>
-  </si>
-  <si>
-    <t>A person with a  formal responsibility in the provisioning of healthcare or related services | Prestataire de santé</t>
-  </si>
-  <si>
-    <t>A person who is directly or indirectly involved in the provisioning of healthcare | Un professionnel impliqué directement ou indirectement dans la prise en charge d'une personne.</t>
   </si>
   <si>
     <t>Bundle.entry:practitioner.search</t>
@@ -2112,7 +2108,7 @@
     <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="118.84375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="95.953125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -30146,10 +30142,10 @@
         <v>507</v>
       </c>
       <c r="L247" t="s" s="2">
-        <v>470</v>
+        <v>508</v>
       </c>
       <c r="M247" t="s" s="2">
-        <v>471</v>
+        <v>509</v>
       </c>
       <c r="N247" s="2"/>
       <c r="O247" s="2"/>
@@ -30229,7 +30225,7 @@
     </row>
     <row r="248">
       <c r="A248" t="s" s="2">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B248" t="s" s="2">
         <v>202</v>
@@ -30341,7 +30337,7 @@
     </row>
     <row r="249">
       <c r="A249" t="s" s="2">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B249" t="s" s="2">
         <v>206</v>
@@ -30453,7 +30449,7 @@
     </row>
     <row r="250">
       <c r="A250" t="s" s="2">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B250" t="s" s="2">
         <v>207</v>
@@ -30567,7 +30563,7 @@
     </row>
     <row r="251">
       <c r="A251" t="s" s="2">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B251" t="s" s="2">
         <v>208</v>
@@ -30683,7 +30679,7 @@
     </row>
     <row r="252">
       <c r="A252" t="s" s="2">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B252" t="s" s="2">
         <v>209</v>
@@ -30797,7 +30793,7 @@
     </row>
     <row r="253">
       <c r="A253" t="s" s="2">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B253" t="s" s="2">
         <v>215</v>
@@ -30911,7 +30907,7 @@
     </row>
     <row r="254">
       <c r="A254" t="s" s="2">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B254" t="s" s="2">
         <v>220</v>
@@ -31023,7 +31019,7 @@
     </row>
     <row r="255">
       <c r="A255" t="s" s="2">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B255" t="s" s="2">
         <v>224</v>
@@ -31135,7 +31131,7 @@
     </row>
     <row r="256">
       <c r="A256" t="s" s="2">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B256" t="s" s="2">
         <v>225</v>
@@ -31249,7 +31245,7 @@
     </row>
     <row r="257">
       <c r="A257" t="s" s="2">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B257" t="s" s="2">
         <v>226</v>
@@ -31365,7 +31361,7 @@
     </row>
     <row r="258">
       <c r="A258" t="s" s="2">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B258" t="s" s="2">
         <v>227</v>
@@ -31479,7 +31475,7 @@
     </row>
     <row r="259">
       <c r="A259" t="s" s="2">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B259" t="s" s="2">
         <v>232</v>
@@ -31593,7 +31589,7 @@
     </row>
     <row r="260">
       <c r="A260" t="s" s="2">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B260" t="s" s="2">
         <v>236</v>
@@ -31707,7 +31703,7 @@
     </row>
     <row r="261">
       <c r="A261" t="s" s="2">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B261" t="s" s="2">
         <v>239</v>
@@ -31821,7 +31817,7 @@
     </row>
     <row r="262">
       <c r="A262" t="s" s="2">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B262" t="s" s="2">
         <v>242</v>
@@ -31935,7 +31931,7 @@
     </row>
     <row r="263">
       <c r="A263" t="s" s="2">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B263" t="s" s="2">
         <v>245</v>
@@ -32049,7 +32045,7 @@
     </row>
     <row r="264">
       <c r="A264" t="s" s="2">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B264" t="s" s="2">
         <v>248</v>
@@ -32161,7 +32157,7 @@
     </row>
     <row r="265">
       <c r="A265" t="s" s="2">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B265" t="s" s="2">
         <v>252</v>
@@ -32273,7 +32269,7 @@
     </row>
     <row r="266">
       <c r="A266" t="s" s="2">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B266" t="s" s="2">
         <v>253</v>
@@ -32387,7 +32383,7 @@
     </row>
     <row r="267">
       <c r="A267" t="s" s="2">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B267" t="s" s="2">
         <v>254</v>
@@ -32503,7 +32499,7 @@
     </row>
     <row r="268">
       <c r="A268" t="s" s="2">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B268" t="s" s="2">
         <v>255</v>
@@ -32617,7 +32613,7 @@
     </row>
     <row r="269">
       <c r="A269" t="s" s="2">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="B269" t="s" s="2">
         <v>258</v>
@@ -32731,7 +32727,7 @@
     </row>
     <row r="270">
       <c r="A270" t="s" s="2">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B270" t="s" s="2">
         <v>261</v>
@@ -32845,7 +32841,7 @@
     </row>
     <row r="271">
       <c r="A271" t="s" s="2">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="B271" t="s" s="2">
         <v>265</v>
@@ -32959,7 +32955,7 @@
     </row>
     <row r="272">
       <c r="A272" t="s" s="2">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B272" t="s" s="2">
         <v>269</v>
@@ -33073,13 +33069,13 @@
     </row>
     <row r="273">
       <c r="A273" t="s" s="2">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="B273" t="s" s="2">
         <v>182</v>
       </c>
       <c r="C273" t="s" s="2">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="D273" t="s" s="2">
         <v>76</v>
@@ -33187,7 +33183,7 @@
     </row>
     <row r="274">
       <c r="A274" t="s" s="2">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B274" t="s" s="2">
         <v>187</v>
@@ -33299,7 +33295,7 @@
     </row>
     <row r="275">
       <c r="A275" t="s" s="2">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B275" t="s" s="2">
         <v>188</v>
@@ -33413,7 +33409,7 @@
     </row>
     <row r="276">
       <c r="A276" t="s" s="2">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B276" t="s" s="2">
         <v>189</v>
@@ -33529,7 +33525,7 @@
     </row>
     <row r="277">
       <c r="A277" t="s" s="2">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B277" t="s" s="2">
         <v>190</v>
@@ -33641,7 +33637,7 @@
     </row>
     <row r="278">
       <c r="A278" t="s" s="2">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B278" t="s" s="2">
         <v>193</v>
@@ -33755,7 +33751,7 @@
     </row>
     <row r="279">
       <c r="A279" t="s" s="2">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B279" t="s" s="2">
         <v>197</v>
@@ -33766,7 +33762,7 @@
       </c>
       <c r="E279" s="2"/>
       <c r="F279" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G279" t="s" s="2">
         <v>86</v>
@@ -33778,16 +33774,16 @@
         <v>76</v>
       </c>
       <c r="J279" t="s" s="2">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="K279" t="s" s="2">
-        <v>541</v>
+        <v>198</v>
       </c>
       <c r="L279" t="s" s="2">
-        <v>542</v>
+        <v>199</v>
       </c>
       <c r="M279" t="s" s="2">
-        <v>543</v>
+        <v>200</v>
       </c>
       <c r="N279" s="2"/>
       <c r="O279" s="2"/>
@@ -33850,13 +33846,13 @@
         <v>76</v>
       </c>
       <c r="AJ279" t="s" s="2">
-        <v>284</v>
+        <v>76</v>
       </c>
       <c r="AK279" t="s" s="2">
-        <v>472</v>
+        <v>76</v>
       </c>
       <c r="AL279" t="s" s="2">
-        <v>473</v>
+        <v>201</v>
       </c>
       <c r="AM279" t="s" s="2">
         <v>76</v>
@@ -33867,7 +33863,7 @@
     </row>
     <row r="280">
       <c r="A280" t="s" s="2">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B280" t="s" s="2">
         <v>202</v>
@@ -33979,7 +33975,7 @@
     </row>
     <row r="281">
       <c r="A281" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B281" t="s" s="2">
         <v>206</v>
@@ -34091,7 +34087,7 @@
     </row>
     <row r="282">
       <c r="A282" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B282" t="s" s="2">
         <v>207</v>
@@ -34205,7 +34201,7 @@
     </row>
     <row r="283">
       <c r="A283" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B283" t="s" s="2">
         <v>208</v>
@@ -34321,7 +34317,7 @@
     </row>
     <row r="284">
       <c r="A284" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B284" t="s" s="2">
         <v>209</v>
@@ -34367,7 +34363,7 @@
         <v>76</v>
       </c>
       <c r="S284" t="s" s="2">
-        <v>330</v>
+        <v>76</v>
       </c>
       <c r="T284" t="s" s="2">
         <v>76</v>
@@ -34435,7 +34431,7 @@
     </row>
     <row r="285">
       <c r="A285" t="s" s="2">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B285" t="s" s="2">
         <v>215</v>
@@ -34549,7 +34545,7 @@
     </row>
     <row r="286">
       <c r="A286" t="s" s="2">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B286" t="s" s="2">
         <v>220</v>
@@ -34563,7 +34559,7 @@
         <v>77</v>
       </c>
       <c r="G286" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="H286" t="s" s="2">
         <v>76</v>
@@ -34661,7 +34657,7 @@
     </row>
     <row r="287">
       <c r="A287" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B287" t="s" s="2">
         <v>224</v>
@@ -34773,7 +34769,7 @@
     </row>
     <row r="288">
       <c r="A288" t="s" s="2">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B288" t="s" s="2">
         <v>225</v>
@@ -34887,7 +34883,7 @@
     </row>
     <row r="289">
       <c r="A289" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B289" t="s" s="2">
         <v>226</v>
@@ -35003,7 +34999,7 @@
     </row>
     <row r="290">
       <c r="A290" t="s" s="2">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B290" t="s" s="2">
         <v>227</v>
@@ -35117,7 +35113,7 @@
     </row>
     <row r="291">
       <c r="A291" t="s" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B291" t="s" s="2">
         <v>232</v>
@@ -35231,7 +35227,7 @@
     </row>
     <row r="292">
       <c r="A292" t="s" s="2">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B292" t="s" s="2">
         <v>236</v>
@@ -35345,7 +35341,7 @@
     </row>
     <row r="293">
       <c r="A293" t="s" s="2">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B293" t="s" s="2">
         <v>239</v>
@@ -35459,7 +35455,7 @@
     </row>
     <row r="294">
       <c r="A294" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B294" t="s" s="2">
         <v>242</v>
@@ -35573,7 +35569,7 @@
     </row>
     <row r="295">
       <c r="A295" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B295" t="s" s="2">
         <v>245</v>
@@ -35687,7 +35683,7 @@
     </row>
     <row r="296">
       <c r="A296" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B296" t="s" s="2">
         <v>248</v>
@@ -35701,7 +35697,7 @@
         <v>77</v>
       </c>
       <c r="G296" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="H296" t="s" s="2">
         <v>76</v>
@@ -35799,7 +35795,7 @@
     </row>
     <row r="297">
       <c r="A297" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B297" t="s" s="2">
         <v>252</v>
@@ -35911,7 +35907,7 @@
     </row>
     <row r="298">
       <c r="A298" t="s" s="2">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B298" t="s" s="2">
         <v>253</v>
@@ -36025,7 +36021,7 @@
     </row>
     <row r="299">
       <c r="A299" t="s" s="2">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B299" t="s" s="2">
         <v>254</v>
@@ -36141,7 +36137,7 @@
     </row>
     <row r="300">
       <c r="A300" t="s" s="2">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B300" t="s" s="2">
         <v>255</v>
@@ -36255,7 +36251,7 @@
     </row>
     <row r="301">
       <c r="A301" t="s" s="2">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B301" t="s" s="2">
         <v>258</v>
@@ -36369,7 +36365,7 @@
     </row>
     <row r="302">
       <c r="A302" t="s" s="2">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B302" t="s" s="2">
         <v>261</v>
@@ -36483,7 +36479,7 @@
     </row>
     <row r="303">
       <c r="A303" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B303" t="s" s="2">
         <v>265</v>
@@ -36597,7 +36593,7 @@
     </row>
     <row r="304">
       <c r="A304" t="s" s="2">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B304" t="s" s="2">
         <v>269</v>
@@ -36711,10 +36707,10 @@
     </row>
     <row r="305">
       <c r="A305" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B305" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C305" s="2"/>
       <c r="D305" t="s" s="2">
@@ -36737,19 +36733,19 @@
         <v>87</v>
       </c>
       <c r="K305" t="s" s="2">
+        <v>569</v>
+      </c>
+      <c r="L305" t="s" s="2">
         <v>570</v>
       </c>
-      <c r="L305" t="s" s="2">
+      <c r="M305" t="s" s="2">
         <v>571</v>
       </c>
-      <c r="M305" t="s" s="2">
+      <c r="N305" t="s" s="2">
         <v>572</v>
       </c>
-      <c r="N305" t="s" s="2">
+      <c r="O305" t="s" s="2">
         <v>573</v>
-      </c>
-      <c r="O305" t="s" s="2">
-        <v>574</v>
       </c>
       <c r="P305" t="s" s="2">
         <v>76</v>
@@ -36798,7 +36794,7 @@
         <v>76</v>
       </c>
       <c r="AF305" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AG305" t="s" s="2">
         <v>77</v>

</xml_diff>